<commit_message>
v3 - first push, refactor, added postgresdb remote db, new api calls, and service impl
</commit_message>
<xml_diff>
--- a/productList.xlsx
+++ b/productList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="192" yWindow="48" windowWidth="19896" windowHeight="9216"/>
+    <workbookView xWindow="190" yWindow="54" windowWidth="19902" windowHeight="9211"/>
   </bookViews>
   <sheets>
     <sheet name="Dane" sheetId="1" r:id="rId1"/>
@@ -47,18 +47,6 @@
     <t>L-duzy</t>
   </si>
   <si>
-    <t>cost-S</t>
-  </si>
-  <si>
-    <t>cost-M</t>
-  </si>
-  <si>
-    <t>cost-L</t>
-  </si>
-  <si>
-    <t>cost-U</t>
-  </si>
-  <si>
     <t>U-rozmiar 'uniwersalny', czyli jeden rozmiar</t>
   </si>
   <si>
@@ -270,6 +258,18 @@
   </si>
   <si>
     <t>PICANTE + CISOWIANKA BEZ GAZU 0,5L</t>
+  </si>
+  <si>
+    <t>costS</t>
+  </si>
+  <si>
+    <t>costM</t>
+  </si>
+  <si>
+    <t>costL</t>
+  </si>
+  <si>
+    <t>costU</t>
   </si>
 </sst>
 </file>
@@ -625,16 +625,16 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.6"/>
   <cols>
-    <col min="1" max="1" width="3.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.8984375" customWidth="1"/>
-    <col min="5" max="5" width="7.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.88671875" customWidth="1"/>
+    <col min="5" max="5" width="7.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -651,16 +651,16 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="H1" t="s">
-        <v>13</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -671,10 +671,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E2" s="5">
         <v>20</v>
@@ -686,7 +686,7 @@
         <v>34.5</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -697,10 +697,10 @@
         <v>0</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E3" s="5">
         <v>21</v>
@@ -712,7 +712,7 @@
         <v>36</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -723,10 +723,10 @@
         <v>0</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E4" s="5">
         <v>23</v>
@@ -738,7 +738,7 @@
         <v>38.5</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -749,10 +749,10 @@
         <v>0</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E5" s="5">
         <v>23</v>
@@ -764,7 +764,7 @@
         <v>38.5</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -775,10 +775,10 @@
         <v>0</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E6" s="5">
         <v>23</v>
@@ -790,7 +790,7 @@
         <v>38.5</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -801,10 +801,10 @@
         <v>0</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E7" s="5">
         <v>23</v>
@@ -816,7 +816,7 @@
         <v>38.5</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -827,10 +827,10 @@
         <v>0</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E8" s="5">
         <v>24.5</v>
@@ -842,7 +842,7 @@
         <v>40</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -853,10 +853,10 @@
         <v>0</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E9" s="5">
         <v>24.5</v>
@@ -868,7 +868,7 @@
         <v>40</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -879,10 +879,10 @@
         <v>0</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E10" s="5">
         <v>26</v>
@@ -894,7 +894,7 @@
         <v>41</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -905,10 +905,10 @@
         <v>0</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E11" s="5">
         <v>26</v>
@@ -920,7 +920,7 @@
         <v>41</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -931,10 +931,10 @@
         <v>0</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E12" s="5">
         <v>27</v>
@@ -946,7 +946,7 @@
         <v>42</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -957,10 +957,10 @@
         <v>0</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E13" s="5">
         <v>26</v>
@@ -972,10 +972,10 @@
         <v>41</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="27.6">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="27.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -983,10 +983,10 @@
         <v>0</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E14" s="5">
         <v>27.5</v>
@@ -998,7 +998,7 @@
         <v>43</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1009,10 +1009,10 @@
         <v>0</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E15" s="5">
         <v>27.5</v>
@@ -1024,7 +1024,7 @@
         <v>43</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1035,10 +1035,10 @@
         <v>0</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E16" s="5">
         <v>28</v>
@@ -1050,10 +1050,10 @@
         <v>44</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="27.6">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1061,10 +1061,10 @@
         <v>0</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E17" s="5">
         <v>28.5</v>
@@ -1076,7 +1076,7 @@
         <v>45</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1087,10 +1087,10 @@
         <v>0</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E18" s="5">
         <v>27.5</v>
@@ -1102,10 +1102,10 @@
         <v>43</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="27.6">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1113,10 +1113,10 @@
         <v>0</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E19" s="5">
         <v>27.5</v>
@@ -1128,7 +1128,7 @@
         <v>43</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1139,10 +1139,10 @@
         <v>0</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E20" s="5">
         <v>27.5</v>
@@ -1154,10 +1154,10 @@
         <v>43</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="27.6">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="27.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1165,10 +1165,10 @@
         <v>0</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E21" s="5">
         <v>27.5</v>
@@ -1180,7 +1180,7 @@
         <v>43</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1191,10 +1191,10 @@
         <v>0</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E22" s="5">
         <v>25</v>
@@ -1206,7 +1206,7 @@
         <v>40</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1217,10 +1217,10 @@
         <v>0</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E23" s="5">
         <v>26</v>
@@ -1232,7 +1232,7 @@
         <v>40</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1243,10 +1243,10 @@
         <v>0</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E24" s="5">
         <v>27.5</v>
@@ -1258,10 +1258,10 @@
         <v>42</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="27.6">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1269,10 +1269,10 @@
         <v>0</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E25" s="5">
         <v>28</v>
@@ -1284,7 +1284,7 @@
         <v>43</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1295,17 +1295,17 @@
         <v>1</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F26" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G26" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H26" s="6">
         <v>7</v>
@@ -1319,17 +1319,17 @@
         <v>1</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F27" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G27" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H27" s="6">
         <v>7</v>
@@ -1343,16 +1343,16 @@
         <v>1</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E28" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F28" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G28" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H28" s="6">
         <v>7</v>
@@ -1366,16 +1366,16 @@
         <v>1</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E29" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F29" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G29" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H29" s="6">
         <v>5</v>
@@ -1389,16 +1389,16 @@
         <v>1</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E30" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F30" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G30" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H30" s="6">
         <v>5</v>
@@ -1412,16 +1412,16 @@
         <v>1</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E31" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F31" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G31" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H31" s="5">
         <v>5</v>
@@ -1435,16 +1435,16 @@
         <v>1</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E32" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F32" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G32" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H32" s="6">
         <v>4</v>
@@ -1458,16 +1458,16 @@
         <v>1</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E33" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F33" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G33" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H33" s="6">
         <v>4</v>
@@ -1481,19 +1481,19 @@
         <v>2</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D34" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E34" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F34" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G34" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H34" s="6">
         <v>40</v>
@@ -1507,19 +1507,19 @@
         <v>2</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D35" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E35" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F35" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G35" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H35" s="6">
         <v>48</v>
@@ -1533,25 +1533,25 @@
         <v>2</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D36" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E36" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F36" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G36" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H36" s="6">
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="27.6">
+    <row r="37" spans="1:8" ht="27.2">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -1559,19 +1559,19 @@
         <v>2</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D37" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E37" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F37" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G37" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H37" s="6">
         <v>38</v>
@@ -1585,19 +1585,19 @@
         <v>2</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D38" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E38" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F38" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G38" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H38" s="6">
         <v>39</v>
@@ -1635,11 +1635,11 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.6"/>
   <cols>
-    <col min="1" max="1" width="9.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="13.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1656,12 +1656,12 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
@@ -1673,7 +1673,7 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1685,10 +1685,10 @@
     <row r="5" spans="1:6">
       <c r="B5" s="1"/>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1711,12 +1711,12 @@
     </row>
     <row r="9" spans="1:6">
       <c r="F9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="F11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>